<commit_message>
Almost finished lab 4.4.3 in physics course. Need to do calculations in point 1 to find the angle of the prisme.
</commit_message>
<xml_diff>
--- a/Physics/4.4.3/4.4.3.xlsx
+++ b/Physics/4.4.3/4.4.3.xlsx
@@ -8,24 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MIPT-MIPS\Labs\Physics\4.4.3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{438ABABA-895B-499A-9AED-E7D339D8053A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E1A38A4-0DAF-4EA9-8C64-462D7A6E64B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32280" yWindow="3345" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Диаграмма1" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
   <si>
     <t>Измерение преломляющего угла</t>
   </si>
@@ -95,12 +104,43 @@
   <si>
     <t>a, см</t>
   </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <r>
+      <t>λ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14.3"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>нм</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="167" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -115,6 +155,12 @@
       <family val="2"/>
       <charset val="204"/>
     </font>
+    <font>
+      <sz val="14.3"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -124,7 +170,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -132,13 +178,75 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -154,6 +262,809 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="639309711"/>
+        <c:axId val="639308463"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="639309711"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="639308463"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="639308463"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="639309711"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ru-RU"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{537AB91A-F967-47E9-9FCE-E19A1F855E4D}">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="67" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="13008022" cy="9439701"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Диаграмма 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{85DDFBEA-095B-4C51-9046-FE4EFD04DB3A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -419,10 +1330,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:O17"/>
+  <dimension ref="B1:O48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -447,141 +1358,143 @@
       </c>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="H4" t="s">
+      <c r="G4" s="2"/>
+      <c r="H4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="3">
         <v>1</v>
       </c>
-      <c r="K4">
+      <c r="K4" s="3">
         <v>2</v>
       </c>
-      <c r="L4">
+      <c r="L4" s="3">
         <v>3</v>
       </c>
-      <c r="M4">
+      <c r="M4" s="3">
         <v>4</v>
       </c>
-      <c r="N4">
+      <c r="N4" s="3">
         <v>5</v>
       </c>
-      <c r="O4">
+      <c r="O4" s="3">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="H5" t="s">
+      <c r="G5" s="4"/>
+      <c r="H5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="K5" t="s">
+      <c r="K5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="L5" t="s">
+      <c r="L5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="M5" t="s">
+      <c r="M5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="N5" t="s">
+      <c r="N5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="O5" t="s">
+      <c r="O5" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="G6" t="s">
+      <c r="G6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="3">
         <v>128</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="3">
         <v>128</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="3">
         <v>127</v>
       </c>
-      <c r="K6">
+      <c r="K6" s="3">
         <v>127</v>
       </c>
-      <c r="L6">
+      <c r="L6" s="3">
         <v>127</v>
       </c>
-      <c r="M6">
+      <c r="M6" s="3">
         <v>126</v>
       </c>
-      <c r="N6">
+      <c r="N6" s="3">
         <v>125</v>
       </c>
-      <c r="O6">
+      <c r="O6" s="3">
         <v>124</v>
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="G7" t="s">
+      <c r="G7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="3">
         <v>47</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="3">
         <v>21</v>
       </c>
-      <c r="J7">
+      <c r="J7" s="3">
         <v>58</v>
       </c>
-      <c r="K7">
+      <c r="K7" s="3">
         <v>57</v>
       </c>
-      <c r="L7">
+      <c r="L7" s="3">
         <v>37</v>
       </c>
-      <c r="M7">
+      <c r="M7" s="3">
         <v>53</v>
       </c>
-      <c r="N7">
+      <c r="N7" s="3">
         <v>41</v>
       </c>
-      <c r="O7">
+      <c r="O7" s="3">
         <v>41</v>
       </c>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="G8" t="s">
+      <c r="G8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="3">
         <v>22</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="3">
         <v>8</v>
       </c>
-      <c r="J8">
+      <c r="J8" s="3">
         <v>37</v>
       </c>
-      <c r="K8">
+      <c r="K8" s="3">
         <v>18</v>
       </c>
-      <c r="L8">
+      <c r="L8" s="3">
         <v>30</v>
       </c>
-      <c r="M8">
+      <c r="M8" s="3">
         <v>15</v>
       </c>
-      <c r="N8">
+      <c r="N8" s="3">
         <v>31</v>
       </c>
-      <c r="O8">
+      <c r="O8" s="3">
         <v>20</v>
       </c>
     </row>
@@ -650,7 +1563,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="17" spans="7:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="5:14" x14ac:dyDescent="0.35">
       <c r="G17" t="s">
         <v>18</v>
       </c>
@@ -658,7 +1571,474 @@
         <v>7.2</v>
       </c>
     </row>
+    <row r="21" spans="5:14" x14ac:dyDescent="0.35">
+      <c r="F21" s="5"/>
+      <c r="G21" s="5" t="str">
+        <f>H4</f>
+        <v>К1</v>
+      </c>
+      <c r="H21" s="5" t="str">
+        <f t="shared" ref="H21:N22" si="0">I4</f>
+        <v>К2</v>
+      </c>
+      <c r="I21" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J21" s="5">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="K21" s="5">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="L21" s="5">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="M21" s="5">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="N21" s="5">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="5:14" x14ac:dyDescent="0.35">
+      <c r="F22" s="5"/>
+      <c r="G22" s="5" t="str">
+        <f>H5</f>
+        <v>красн</v>
+      </c>
+      <c r="H22" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>красн</v>
+      </c>
+      <c r="I22" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>желт</v>
+      </c>
+      <c r="J22" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>желт</v>
+      </c>
+      <c r="K22" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>зелен</v>
+      </c>
+      <c r="L22" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>голуб</v>
+      </c>
+      <c r="M22" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>синий</v>
+      </c>
+      <c r="N22" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>фиолет</v>
+      </c>
+    </row>
+    <row r="23" spans="5:14" x14ac:dyDescent="0.35">
+      <c r="F23" s="5" t="str">
+        <f>G6</f>
+        <v>градусы</v>
+      </c>
+      <c r="G23" s="5">
+        <f>179-H6</f>
+        <v>51</v>
+      </c>
+      <c r="H23" s="5">
+        <f t="shared" ref="H23:N23" si="1">179-I6</f>
+        <v>51</v>
+      </c>
+      <c r="I23" s="5">
+        <f t="shared" si="1"/>
+        <v>52</v>
+      </c>
+      <c r="J23" s="5">
+        <f t="shared" si="1"/>
+        <v>52</v>
+      </c>
+      <c r="K23" s="5">
+        <f t="shared" si="1"/>
+        <v>52</v>
+      </c>
+      <c r="L23" s="5">
+        <f t="shared" si="1"/>
+        <v>53</v>
+      </c>
+      <c r="M23" s="5">
+        <f t="shared" si="1"/>
+        <v>54</v>
+      </c>
+      <c r="N23" s="5">
+        <f t="shared" si="1"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="5:14" x14ac:dyDescent="0.35">
+      <c r="F24" s="5" t="str">
+        <f t="shared" ref="F24:F25" si="2">G7</f>
+        <v>минуты</v>
+      </c>
+      <c r="G24" s="5">
+        <f>59-H7</f>
+        <v>12</v>
+      </c>
+      <c r="H24" s="5">
+        <f t="shared" ref="H24:N24" si="3">59-I7</f>
+        <v>38</v>
+      </c>
+      <c r="I24" s="5">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="J24" s="5">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="K24" s="5">
+        <f t="shared" si="3"/>
+        <v>22</v>
+      </c>
+      <c r="L24" s="5">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="M24" s="5">
+        <f t="shared" si="3"/>
+        <v>18</v>
+      </c>
+      <c r="N24" s="5">
+        <f t="shared" si="3"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="5:14" x14ac:dyDescent="0.35">
+      <c r="F25" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v>секнды</v>
+      </c>
+      <c r="G25" s="5">
+        <f>60-H8</f>
+        <v>38</v>
+      </c>
+      <c r="H25" s="5">
+        <f t="shared" ref="H25:N25" si="4">60-I8</f>
+        <v>52</v>
+      </c>
+      <c r="I25" s="5">
+        <f t="shared" si="4"/>
+        <v>23</v>
+      </c>
+      <c r="J25" s="5">
+        <f t="shared" si="4"/>
+        <v>42</v>
+      </c>
+      <c r="K25" s="5">
+        <f t="shared" si="4"/>
+        <v>30</v>
+      </c>
+      <c r="L25" s="5">
+        <f t="shared" si="4"/>
+        <v>45</v>
+      </c>
+      <c r="M25" s="5">
+        <f t="shared" si="4"/>
+        <v>29</v>
+      </c>
+      <c r="N25" s="5">
+        <f t="shared" si="4"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" spans="5:14" x14ac:dyDescent="0.35">
+      <c r="E29">
+        <v>59</v>
+      </c>
+      <c r="G29">
+        <f>(G23+$E$29)/2</f>
+        <v>55</v>
+      </c>
+      <c r="H29">
+        <f t="shared" ref="H29:N29" si="5">(H23+$E$29)/2</f>
+        <v>55</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="5"/>
+        <v>55.5</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="5"/>
+        <v>55.5</v>
+      </c>
+      <c r="K29">
+        <f t="shared" si="5"/>
+        <v>55.5</v>
+      </c>
+      <c r="L29">
+        <f t="shared" si="5"/>
+        <v>56</v>
+      </c>
+      <c r="M29">
+        <f t="shared" si="5"/>
+        <v>56.5</v>
+      </c>
+      <c r="N29">
+        <f t="shared" si="5"/>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="5:14" x14ac:dyDescent="0.35">
+      <c r="E30">
+        <v>12</v>
+      </c>
+      <c r="G30">
+        <f>(G24+$E$30)/2</f>
+        <v>12</v>
+      </c>
+      <c r="H30">
+        <f t="shared" ref="H30:N30" si="6">(H24+$E$30)/2</f>
+        <v>25</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="6"/>
+        <v>6.5</v>
+      </c>
+      <c r="J30">
+        <f t="shared" si="6"/>
+        <v>7</v>
+      </c>
+      <c r="K30">
+        <f t="shared" si="6"/>
+        <v>17</v>
+      </c>
+      <c r="L30">
+        <f t="shared" si="6"/>
+        <v>9</v>
+      </c>
+      <c r="M30">
+        <f t="shared" si="6"/>
+        <v>15</v>
+      </c>
+      <c r="N30">
+        <f t="shared" si="6"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="5:14" x14ac:dyDescent="0.35">
+      <c r="E31">
+        <v>16</v>
+      </c>
+      <c r="G31">
+        <f>(G25+$E$31)/2</f>
+        <v>27</v>
+      </c>
+      <c r="H31">
+        <f t="shared" ref="H31:N31" si="7">(H25+$E$31)/2</f>
+        <v>34</v>
+      </c>
+      <c r="I31">
+        <f t="shared" si="7"/>
+        <v>19.5</v>
+      </c>
+      <c r="J31">
+        <f t="shared" si="7"/>
+        <v>29</v>
+      </c>
+      <c r="K31">
+        <f t="shared" si="7"/>
+        <v>23</v>
+      </c>
+      <c r="L31">
+        <f t="shared" si="7"/>
+        <v>30.5</v>
+      </c>
+      <c r="M31">
+        <f t="shared" si="7"/>
+        <v>22.5</v>
+      </c>
+      <c r="N31">
+        <f t="shared" si="7"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="33" spans="5:15" x14ac:dyDescent="0.35">
+      <c r="E33">
+        <f>E29/2</f>
+        <v>29.5</v>
+      </c>
+      <c r="G33">
+        <f>G29+G30/60+G31/3600</f>
+        <v>55.207500000000003</v>
+      </c>
+      <c r="H33">
+        <f t="shared" ref="H33:N33" si="8">H29+H30/60+H31/3600</f>
+        <v>55.426111111111112</v>
+      </c>
+      <c r="I33">
+        <f t="shared" si="8"/>
+        <v>55.613750000000003</v>
+      </c>
+      <c r="J33">
+        <f t="shared" si="8"/>
+        <v>55.624722222222225</v>
+      </c>
+      <c r="K33">
+        <f t="shared" si="8"/>
+        <v>55.789722222222217</v>
+      </c>
+      <c r="L33">
+        <f t="shared" si="8"/>
+        <v>56.158472222222223</v>
+      </c>
+      <c r="M33">
+        <f t="shared" si="8"/>
+        <v>56.756250000000001</v>
+      </c>
+      <c r="N33">
+        <f t="shared" si="8"/>
+        <v>57.257777777777775</v>
+      </c>
+    </row>
+    <row r="34" spans="5:15" x14ac:dyDescent="0.35">
+      <c r="E34">
+        <f t="shared" ref="E34:E35" si="9">E30/2</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="5:15" x14ac:dyDescent="0.35">
+      <c r="E35">
+        <f t="shared" si="9"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="5:15" x14ac:dyDescent="0.35">
+      <c r="E37">
+        <f>E33+E34/60+E35/3600</f>
+        <v>29.602222222222224</v>
+      </c>
+      <c r="G37">
+        <f>SIN(G33/180*3.14)</f>
+        <v>0.82094508063509986</v>
+      </c>
+      <c r="H37">
+        <f t="shared" ref="H37:O37" si="10">SIN(H33/180*3.14)</f>
+        <v>0.82311666979208342</v>
+      </c>
+      <c r="I37">
+        <f t="shared" si="10"/>
+        <v>0.82497104846391633</v>
+      </c>
+      <c r="J37">
+        <f t="shared" si="10"/>
+        <v>0.82507921028677433</v>
+      </c>
+      <c r="K37">
+        <f t="shared" si="10"/>
+        <v>0.82670209771949521</v>
+      </c>
+      <c r="L37">
+        <f t="shared" si="10"/>
+        <v>0.83030422804309822</v>
+      </c>
+      <c r="M37">
+        <f t="shared" si="10"/>
+        <v>0.83607055689210485</v>
+      </c>
+      <c r="N37">
+        <f t="shared" si="10"/>
+        <v>0.84083832213498888</v>
+      </c>
+      <c r="O37">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="5:15" x14ac:dyDescent="0.35">
+      <c r="G39">
+        <f>SIN(E37/180*3.14)</f>
+        <v>0.49374783727496097</v>
+      </c>
+    </row>
+    <row r="41" spans="5:15" x14ac:dyDescent="0.35">
+      <c r="F41" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G41" s="6">
+        <f>G37/$G$39</f>
+        <v>1.6626808639121744</v>
+      </c>
+      <c r="H41" s="6">
+        <f t="shared" ref="H41:N41" si="11">H37/$G$39</f>
+        <v>1.6670790384317202</v>
+      </c>
+      <c r="I41" s="6">
+        <f t="shared" si="11"/>
+        <v>1.6708347585216905</v>
+      </c>
+      <c r="J41" s="6">
+        <f t="shared" si="11"/>
+        <v>1.6710538214009427</v>
+      </c>
+      <c r="K41" s="6">
+        <f t="shared" si="11"/>
+        <v>1.6743406964213534</v>
+      </c>
+      <c r="L41" s="6">
+        <f t="shared" si="11"/>
+        <v>1.6816361821970147</v>
+      </c>
+      <c r="M41" s="6">
+        <f t="shared" si="11"/>
+        <v>1.6933148740589001</v>
+      </c>
+      <c r="N41" s="6">
+        <f t="shared" si="11"/>
+        <v>1.7029711497586537</v>
+      </c>
+    </row>
+    <row r="42" spans="5:15" ht="19" x14ac:dyDescent="0.35">
+      <c r="F42" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G42" s="8">
+        <v>690.7</v>
+      </c>
+      <c r="H42" s="8">
+        <v>623.4</v>
+      </c>
+      <c r="I42" s="8">
+        <v>579.1</v>
+      </c>
+      <c r="J42" s="8">
+        <v>577</v>
+      </c>
+      <c r="K42" s="8">
+        <v>546.1</v>
+      </c>
+      <c r="L42" s="8">
+        <v>491.6</v>
+      </c>
+      <c r="M42" s="8">
+        <v>435.8</v>
+      </c>
+      <c r="N42" s="8">
+        <v>404.7</v>
+      </c>
+    </row>
+    <row r="48" spans="5:15" x14ac:dyDescent="0.35">
+      <c r="J48">
+        <v>0.2</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="G4:G5"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Added labs 77 in RC and 4.3.1in Physics
</commit_message>
<xml_diff>
--- a/Physics/4.4.3/4.4.3.xlsx
+++ b/Physics/4.4.3/4.4.3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MIPT-MIPS\Labs\Physics\4.4.3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E1A38A4-0DAF-4EA9-8C64-462D7A6E64B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B813F699-BF8E-4B82-9834-351B0D6782C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32280" yWindow="3345" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="380" yWindow="380" windowWidth="16200" windowHeight="9970" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Диаграмма1" sheetId="2" r:id="rId1"/>
@@ -137,8 +137,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="166" formatCode="0.0000"/>
-    <numFmt numFmtId="167" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -226,26 +226,26 @@
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1332,8 +1332,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:O48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1358,143 +1358,143 @@
       </c>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="G4" s="2"/>
-      <c r="H4" s="3" t="s">
+      <c r="G4" s="7"/>
+      <c r="H4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="J4" s="3">
+      <c r="J4" s="2">
         <v>1</v>
       </c>
-      <c r="K4" s="3">
+      <c r="K4" s="2">
         <v>2</v>
       </c>
-      <c r="L4" s="3">
+      <c r="L4" s="2">
         <v>3</v>
       </c>
-      <c r="M4" s="3">
+      <c r="M4" s="2">
         <v>4</v>
       </c>
-      <c r="N4" s="3">
+      <c r="N4" s="2">
         <v>5</v>
       </c>
-      <c r="O4" s="3">
+      <c r="O4" s="2">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="G5" s="4"/>
-      <c r="H5" s="3" t="s">
+      <c r="G5" s="8"/>
+      <c r="H5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="I5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="J5" s="3" t="s">
+      <c r="J5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="K5" s="3" t="s">
+      <c r="K5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="L5" s="3" t="s">
+      <c r="L5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="M5" s="3" t="s">
+      <c r="M5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="N5" s="3" t="s">
+      <c r="N5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="O5" s="3" t="s">
+      <c r="O5" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="G6" s="3" t="s">
+      <c r="G6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="2">
         <v>128</v>
       </c>
-      <c r="I6" s="3">
+      <c r="I6" s="2">
         <v>128</v>
       </c>
-      <c r="J6" s="3">
+      <c r="J6" s="2">
         <v>127</v>
       </c>
-      <c r="K6" s="3">
+      <c r="K6" s="2">
         <v>127</v>
       </c>
-      <c r="L6" s="3">
+      <c r="L6" s="2">
         <v>127</v>
       </c>
-      <c r="M6" s="3">
+      <c r="M6" s="2">
         <v>126</v>
       </c>
-      <c r="N6" s="3">
+      <c r="N6" s="2">
         <v>125</v>
       </c>
-      <c r="O6" s="3">
+      <c r="O6" s="2">
         <v>124</v>
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="G7" s="3" t="s">
+      <c r="G7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7" s="2">
         <v>47</v>
       </c>
-      <c r="I7" s="3">
+      <c r="I7" s="2">
         <v>21</v>
       </c>
-      <c r="J7" s="3">
+      <c r="J7" s="2">
         <v>58</v>
       </c>
-      <c r="K7" s="3">
+      <c r="K7" s="2">
         <v>57</v>
       </c>
-      <c r="L7" s="3">
+      <c r="L7" s="2">
         <v>37</v>
       </c>
-      <c r="M7" s="3">
+      <c r="M7" s="2">
         <v>53</v>
       </c>
-      <c r="N7" s="3">
+      <c r="N7" s="2">
         <v>41</v>
       </c>
-      <c r="O7" s="3">
+      <c r="O7" s="2">
         <v>41</v>
       </c>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="G8" s="3" t="s">
+      <c r="G8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H8" s="3">
+      <c r="H8" s="2">
         <v>22</v>
       </c>
-      <c r="I8" s="3">
+      <c r="I8" s="2">
         <v>8</v>
       </c>
-      <c r="J8" s="3">
+      <c r="J8" s="2">
         <v>37</v>
       </c>
-      <c r="K8" s="3">
+      <c r="K8" s="2">
         <v>18</v>
       </c>
-      <c r="L8" s="3">
+      <c r="L8" s="2">
         <v>30</v>
       </c>
-      <c r="M8" s="3">
+      <c r="M8" s="2">
         <v>15</v>
       </c>
-      <c r="N8" s="3">
+      <c r="N8" s="2">
         <v>31</v>
       </c>
-      <c r="O8" s="3">
+      <c r="O8" s="2">
         <v>20</v>
       </c>
     </row>
@@ -1563,7 +1563,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="17" spans="5:14" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:14" x14ac:dyDescent="0.35">
       <c r="G17" t="s">
         <v>18</v>
       </c>
@@ -1571,191 +1571,207 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="21" spans="5:14" x14ac:dyDescent="0.35">
-      <c r="F21" s="5"/>
-      <c r="G21" s="5" t="str">
+    <row r="21" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="F21" s="3"/>
+      <c r="G21" s="3" t="str">
         <f>H4</f>
         <v>К1</v>
       </c>
-      <c r="H21" s="5" t="str">
+      <c r="H21" s="3" t="str">
         <f t="shared" ref="H21:N22" si="0">I4</f>
         <v>К2</v>
       </c>
-      <c r="I21" s="5">
+      <c r="I21" s="3">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="J21" s="5">
+      <c r="J21" s="3">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="K21" s="5">
+      <c r="K21" s="3">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="L21" s="5">
+      <c r="L21" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="M21" s="5">
+      <c r="M21" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="N21" s="5">
+      <c r="N21" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="5:14" x14ac:dyDescent="0.35">
-      <c r="F22" s="5"/>
-      <c r="G22" s="5" t="str">
+    <row r="22" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="F22" s="3"/>
+      <c r="G22" s="3" t="str">
         <f>H5</f>
         <v>красн</v>
       </c>
-      <c r="H22" s="5" t="str">
+      <c r="H22" s="3" t="str">
         <f t="shared" si="0"/>
         <v>красн</v>
       </c>
-      <c r="I22" s="5" t="str">
+      <c r="I22" s="3" t="str">
         <f t="shared" si="0"/>
         <v>желт</v>
       </c>
-      <c r="J22" s="5" t="str">
+      <c r="J22" s="3" t="str">
         <f t="shared" si="0"/>
         <v>желт</v>
       </c>
-      <c r="K22" s="5" t="str">
+      <c r="K22" s="3" t="str">
         <f t="shared" si="0"/>
         <v>зелен</v>
       </c>
-      <c r="L22" s="5" t="str">
+      <c r="L22" s="3" t="str">
         <f t="shared" si="0"/>
         <v>голуб</v>
       </c>
-      <c r="M22" s="5" t="str">
+      <c r="M22" s="3" t="str">
         <f t="shared" si="0"/>
         <v>синий</v>
       </c>
-      <c r="N22" s="5" t="str">
+      <c r="N22" s="3" t="str">
         <f t="shared" si="0"/>
         <v>фиолет</v>
       </c>
     </row>
-    <row r="23" spans="5:14" x14ac:dyDescent="0.35">
-      <c r="F23" s="5" t="str">
+    <row r="23" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B23">
+        <f>I23+I24/60+I25/3600</f>
+        <v>52.023055555555551</v>
+      </c>
+      <c r="C23">
+        <f>J23+J24/60+J25/3600</f>
+        <v>52.044999999999995</v>
+      </c>
+      <c r="F23" s="3" t="str">
         <f>G6</f>
         <v>градусы</v>
       </c>
-      <c r="G23" s="5">
+      <c r="G23" s="3">
         <f>179-H6</f>
         <v>51</v>
       </c>
-      <c r="H23" s="5">
+      <c r="H23" s="3">
         <f t="shared" ref="H23:N23" si="1">179-I6</f>
         <v>51</v>
       </c>
-      <c r="I23" s="5">
+      <c r="I23" s="3">
         <f t="shared" si="1"/>
         <v>52</v>
       </c>
-      <c r="J23" s="5">
+      <c r="J23" s="3">
         <f t="shared" si="1"/>
         <v>52</v>
       </c>
-      <c r="K23" s="5">
+      <c r="K23" s="3">
         <f t="shared" si="1"/>
         <v>52</v>
       </c>
-      <c r="L23" s="5">
+      <c r="L23" s="3">
         <f t="shared" si="1"/>
         <v>53</v>
       </c>
-      <c r="M23" s="5">
+      <c r="M23" s="3">
         <f t="shared" si="1"/>
         <v>54</v>
       </c>
-      <c r="N23" s="5">
+      <c r="N23" s="3">
         <f t="shared" si="1"/>
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="5:14" x14ac:dyDescent="0.35">
-      <c r="F24" s="5" t="str">
+    <row r="24" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="F24" s="3" t="str">
         <f t="shared" ref="F24:F25" si="2">G7</f>
         <v>минуты</v>
       </c>
-      <c r="G24" s="5">
+      <c r="G24" s="3">
         <f>59-H7</f>
         <v>12</v>
       </c>
-      <c r="H24" s="5">
+      <c r="H24" s="3">
         <f t="shared" ref="H24:N24" si="3">59-I7</f>
         <v>38</v>
       </c>
-      <c r="I24" s="5">
+      <c r="I24" s="3">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="J24" s="5">
+      <c r="J24" s="3">
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="K24" s="5">
+      <c r="K24" s="3">
         <f t="shared" si="3"/>
         <v>22</v>
       </c>
-      <c r="L24" s="5">
+      <c r="L24" s="3">
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="M24" s="5">
+      <c r="M24" s="3">
         <f t="shared" si="3"/>
         <v>18</v>
       </c>
-      <c r="N24" s="5">
+      <c r="N24" s="3">
         <f t="shared" si="3"/>
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="5:14" x14ac:dyDescent="0.35">
-      <c r="F25" s="5" t="str">
+    <row r="25" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B25">
+        <f>C23-B23</f>
+        <v>2.1944444444443434E-2</v>
+      </c>
+      <c r="C25">
+        <f>B25/2.1*3.14/180</f>
+        <v>1.8228982951204334E-4</v>
+      </c>
+      <c r="F25" s="3" t="str">
         <f t="shared" si="2"/>
         <v>секнды</v>
       </c>
-      <c r="G25" s="5">
+      <c r="G25" s="3">
         <f>60-H8</f>
         <v>38</v>
       </c>
-      <c r="H25" s="5">
+      <c r="H25" s="3">
         <f t="shared" ref="H25:N25" si="4">60-I8</f>
         <v>52</v>
       </c>
-      <c r="I25" s="5">
+      <c r="I25" s="3">
         <f t="shared" si="4"/>
         <v>23</v>
       </c>
-      <c r="J25" s="5">
+      <c r="J25" s="3">
         <f t="shared" si="4"/>
         <v>42</v>
       </c>
-      <c r="K25" s="5">
+      <c r="K25" s="3">
         <f t="shared" si="4"/>
         <v>30</v>
       </c>
-      <c r="L25" s="5">
+      <c r="L25" s="3">
         <f t="shared" si="4"/>
         <v>45</v>
       </c>
-      <c r="M25" s="5">
+      <c r="M25" s="3">
         <f t="shared" si="4"/>
         <v>29</v>
       </c>
-      <c r="N25" s="5">
+      <c r="N25" s="3">
         <f t="shared" si="4"/>
         <v>40</v>
       </c>
     </row>
-    <row r="29" spans="5:14" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:14" x14ac:dyDescent="0.35">
       <c r="E29">
         <v>59</v>
       </c>
@@ -1792,7 +1808,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="5:14" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:14" x14ac:dyDescent="0.35">
       <c r="E30">
         <v>12</v>
       </c>
@@ -1829,7 +1845,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="5:14" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:14" x14ac:dyDescent="0.35">
       <c r="E31">
         <v>16</v>
       </c>
@@ -1965,68 +1981,68 @@
       </c>
     </row>
     <row r="41" spans="5:15" x14ac:dyDescent="0.35">
-      <c r="F41" s="5" t="s">
+      <c r="F41" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G41" s="6">
+      <c r="G41" s="4">
         <f>G37/$G$39</f>
         <v>1.6626808639121744</v>
       </c>
-      <c r="H41" s="6">
+      <c r="H41" s="4">
         <f t="shared" ref="H41:N41" si="11">H37/$G$39</f>
         <v>1.6670790384317202</v>
       </c>
-      <c r="I41" s="6">
+      <c r="I41" s="4">
         <f t="shared" si="11"/>
         <v>1.6708347585216905</v>
       </c>
-      <c r="J41" s="6">
+      <c r="J41" s="4">
         <f t="shared" si="11"/>
         <v>1.6710538214009427</v>
       </c>
-      <c r="K41" s="6">
+      <c r="K41" s="4">
         <f t="shared" si="11"/>
         <v>1.6743406964213534</v>
       </c>
-      <c r="L41" s="6">
+      <c r="L41" s="4">
         <f t="shared" si="11"/>
         <v>1.6816361821970147</v>
       </c>
-      <c r="M41" s="6">
+      <c r="M41" s="4">
         <f t="shared" si="11"/>
         <v>1.6933148740589001</v>
       </c>
-      <c r="N41" s="6">
+      <c r="N41" s="4">
         <f t="shared" si="11"/>
         <v>1.7029711497586537</v>
       </c>
     </row>
     <row r="42" spans="5:15" ht="19" x14ac:dyDescent="0.35">
-      <c r="F42" s="7" t="s">
+      <c r="F42" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G42" s="8">
+      <c r="G42" s="6">
         <v>690.7</v>
       </c>
-      <c r="H42" s="8">
+      <c r="H42" s="6">
         <v>623.4</v>
       </c>
-      <c r="I42" s="8">
+      <c r="I42" s="6">
         <v>579.1</v>
       </c>
-      <c r="J42" s="8">
+      <c r="J42" s="6">
         <v>577</v>
       </c>
-      <c r="K42" s="8">
+      <c r="K42" s="6">
         <v>546.1</v>
       </c>
-      <c r="L42" s="8">
+      <c r="L42" s="6">
         <v>491.6</v>
       </c>
-      <c r="M42" s="8">
+      <c r="M42" s="6">
         <v>435.8</v>
       </c>
-      <c r="N42" s="8">
+      <c r="N42" s="6">
         <v>404.7</v>
       </c>
     </row>

</xml_diff>